<commit_message>
get_hotels debugging, minor changes to results template
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-27-2023/Susan Rippetoe - Phoenix, Arizona, United States of America.xlsx
+++ b/P2_Performer/Results/03-27-2023/Susan Rippetoe - Phoenix, Arizona, United States of America.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-27-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A10D8941-F0D7-486A-A751-FA88FEA75B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92C927B8-2B1E-420E-AAC1-2C9A2010B413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2004" yWindow="2364" windowWidth="17280" windowHeight="8964" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Hotel</t>
   </si>
@@ -141,18 +141,6 @@
   </si>
   <si>
     <t>Legacy Golf Resort</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Min Temp F</t>
-  </si>
-  <si>
-    <t>Max Temp F</t>
-  </si>
-  <si>
-    <t>Precip</t>
   </si>
 </sst>
 </file>
@@ -713,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,15 +740,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,9 +761,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,15 +780,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1115,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB9D9BD-3947-44C2-BFCC-D5F202797C3B}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,7 +1132,7 @@
       <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="48">
         <v>96</v>
       </c>
       <c r="C2" s="11">
@@ -1163,7 +1148,7 @@
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="49">
         <v>75</v>
       </c>
       <c r="C3" s="8">
@@ -1179,7 +1164,7 @@
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="50">
         <v>96</v>
       </c>
       <c r="C4" s="13">
@@ -1217,34 +1202,34 @@
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
@@ -1261,67 +1246,67 @@
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
@@ -1341,152 +1326,165 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>38</v>
+      <c r="A18" s="51">
+        <v>45208</v>
+      </c>
+      <c r="B18" s="19">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="C18" s="23">
+        <v>88.7</v>
+      </c>
+      <c r="D18" s="19">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="54">
-        <v>45208</v>
+      <c r="A19" s="52">
+        <v>45209</v>
       </c>
       <c r="B19" s="8">
-        <v>67.400000000000006</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="C19" s="8">
-        <v>88.7</v>
+        <v>88.5</v>
       </c>
       <c r="D19" s="7">
-        <v>9.1999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E19" s="9">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="54">
-        <v>45209</v>
+      <c r="A20" s="52">
+        <v>45210</v>
       </c>
       <c r="B20" s="8">
         <v>66.599999999999994</v>
       </c>
       <c r="C20" s="8">
-        <v>88.5</v>
+        <v>89.8</v>
       </c>
       <c r="D20" s="7">
-        <v>8.8000000000000007</v>
+        <v>9.1</v>
       </c>
       <c r="E20" s="9">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="54">
-        <v>45210</v>
+      <c r="A21" s="52">
+        <v>45211</v>
       </c>
       <c r="B21" s="8">
-        <v>66.599999999999994</v>
+        <v>67.7</v>
       </c>
       <c r="C21" s="8">
-        <v>89.8</v>
+        <v>89.5</v>
       </c>
       <c r="D21" s="7">
-        <v>9.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E21" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="54">
-        <v>45211</v>
+      <c r="A22" s="52">
+        <v>45212</v>
       </c>
       <c r="B22" s="8">
-        <v>67.7</v>
+        <v>66.3</v>
       </c>
       <c r="C22" s="8">
-        <v>89.5</v>
+        <v>90.1</v>
       </c>
       <c r="D22" s="7">
-        <v>8.3000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="E22" s="9">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="53">
+        <v>45213</v>
+      </c>
+      <c r="B23" s="5">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5">
+        <v>92.7</v>
+      </c>
+      <c r="D23" s="5">
+        <v>6.7</v>
+      </c>
+      <c r="E23" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="55">
-        <v>45212</v>
-      </c>
-      <c r="B23" s="5">
-        <v>66.3</v>
-      </c>
-      <c r="C23" s="5">
-        <v>90.1</v>
-      </c>
-      <c r="D23" s="5">
-        <v>7.1</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0.11</v>
-      </c>
-    </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="56">
-        <v>45213</v>
-      </c>
-      <c r="B24" s="21">
-        <v>67</v>
-      </c>
-      <c r="C24" s="21">
-        <v>92.7</v>
-      </c>
-      <c r="D24" s="21">
-        <v>6.7</v>
-      </c>
-      <c r="E24" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="27"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1498,6 +1496,11 @@
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>